<commit_message>
fix issue in visual
</commit_message>
<xml_diff>
--- a/visualize_struct_memory_layout.xlsx
+++ b/visualize_struct_memory_layout.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t xml:space="preserve">Struct:</t>
   </si>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">c</t>
   </si>
   <si>
-    <t xml:space="preserve">(this isn’t exactly the struct you showed, but it’s similar)</t>
-  </si>
-  <si>
     <t xml:space="preserve">d</t>
   </si>
   <si>
@@ -58,22 +55,22 @@
     <t xml:space="preserve">f</t>
   </si>
   <si>
+    <t xml:space="preserve">64-bit word size</t>
+  </si>
+  <si>
     <t xml:space="preserve">32-bit word size</t>
   </si>
   <si>
-    <t xml:space="preserve">64-bit word size</t>
+    <t xml:space="preserve">Size: 32 Bytes</t>
   </si>
   <si>
     <t xml:space="preserve">Size: 28 bytes</t>
   </si>
   <si>
-    <t xml:space="preserve">Size: 32 Bytes</t>
+    <t xml:space="preserve">Holes: 7</t>
   </si>
   <si>
     <t xml:space="preserve">Holes: 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holes: 7</t>
   </si>
 </sst>
 </file>
@@ -88,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -183,11 +181,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -209,6 +211,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,283 +302,281 @@
   <dimension ref="B2:N24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="5" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="C16" s="5" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="D16" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="E16" s="5" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="F16" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G16" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="K15" s="2" t="n">
+      <c r="H16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="K16" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="M15" s="3" t="n">
+      <c r="M16" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="N15" s="3" t="n">
+      <c r="N16" s="4" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="G16" s="4" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="F17" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="H17" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="I17" s="8" t="n">
+        <v>23</v>
+      </c>
+      <c r="K17" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="L17" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="I16" s="4" t="n">
+      <c r="M17" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="N17" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="K16" s="5" t="n">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <v>27</v>
+      </c>
+      <c r="F18" s="9" t="n">
+        <v>28</v>
+      </c>
+      <c r="G18" s="9" t="n">
+        <v>29</v>
+      </c>
+      <c r="H18" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="I18" s="9" t="n">
+        <v>31</v>
+      </c>
+      <c r="K18" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="L16" s="5" t="n">
+      <c r="L18" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="M16" s="5" t="n">
+      <c r="M18" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="N16" s="5" t="n">
+      <c r="N18" s="6" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="C17" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="G17" s="5" t="n">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K19" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="H17" s="5" t="n">
+      <c r="L19" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="M19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="N19" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="K17" s="0" t="n">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K20" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L20" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M20" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N20" s="7" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C18" s="5" t="n">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K21" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="L21" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="M21" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="N21" s="7" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="K23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="5" t="n">
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="H18" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="I18" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="J18" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="K18" s="6" t="n">
-        <v>28</v>
-      </c>
-      <c r="L18" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="M18" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="N18" s="6" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5" t="n">
+      <c r="K24" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C19" s="5" t="n">
-        <v>17</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="C20" s="6" t="n">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="E20" s="6" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="C21" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D21" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="E21" s="6" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
investigate #pragma pack(push, 1)
</commit_message>
<xml_diff>
--- a/visualize_struct_memory_layout.xlsx
+++ b/visualize_struct_memory_layout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t xml:space="preserve">Struct:</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t xml:space="preserve">Holes: 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#pragma pack(push, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size: 25 bytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holes: 0</t>
   </si>
 </sst>
 </file>
@@ -181,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,7 +223,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,13 +308,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:N24"/>
+  <dimension ref="B2:N40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O35" activeCellId="0" sqref="O35"/>
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -454,16 +467,16 @@
       <c r="E17" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="F17" s="8" t="n">
+      <c r="F17" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G17" s="8" t="n">
+      <c r="G17" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="H17" s="8" t="n">
+      <c r="H17" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="I17" s="0" t="n">
         <v>23</v>
       </c>
       <c r="K17" s="5" t="n">
@@ -573,6 +586,232 @@
       </c>
       <c r="K24" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="N31" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C32" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="H32" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="I32" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="K32" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L32" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="M32" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="N32" s="5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="C33" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <v>19</v>
+      </c>
+      <c r="F33" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G33" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="H33" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="I33" s="8" t="n">
+        <v>23</v>
+      </c>
+      <c r="K33" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="L33" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="M33" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="N33" s="6" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="C34" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="D34" s="9" t="n">
+        <v>26</v>
+      </c>
+      <c r="E34" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="F34" s="9" t="n">
+        <v>28</v>
+      </c>
+      <c r="G34" s="9" t="n">
+        <v>29</v>
+      </c>
+      <c r="H34" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="I34" s="9" t="n">
+        <v>31</v>
+      </c>
+      <c r="K34" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="L34" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="M34" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="N34" s="6" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K35" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="L35" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="M35" s="7" t="n">
+        <v>18</v>
+      </c>
+      <c r="N35" s="7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K36" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="L36" s="7" t="n">
+        <v>21</v>
+      </c>
+      <c r="M36" s="7" t="n">
+        <v>22</v>
+      </c>
+      <c r="N36" s="7" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K37" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="L37" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="M37" s="9" t="n">
+        <v>26</v>
+      </c>
+      <c r="N37" s="9" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>